<commit_message>
updated project design to one document
</commit_message>
<xml_diff>
--- a/doc/Software Project Requirements.xlsx
+++ b/doc/Software Project Requirements.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/josephsoriano/Desktop/School/2019 Spring/CSE 3310/Project/Superchat/doc/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/josephsoriano/Desktop/School/2019 Spring/CSE 3310/Project/Superchat/doc/Design/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{394C39B5-60A7-9B49-930F-044DB1EA6757}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBA9F500-A057-4246-BF8C-419E14AA0542}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{8E689F70-54D6-C242-BE1D-4E59EC62B863}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="123">
   <si>
     <t>Identifier</t>
   </si>
@@ -71,15 +71,6 @@
     <t>Both</t>
   </si>
   <si>
-    <t>User will have option to sign in as a specific user</t>
-  </si>
-  <si>
-    <t xml:space="preserve">User will have the ability to create chat rooms </t>
-  </si>
-  <si>
-    <t>User will be able to move between chat rooms</t>
-  </si>
-  <si>
     <t>There will be a maximum of 10 chat rooms</t>
   </si>
   <si>
@@ -95,9 +86,6 @@
     <t>The server will support up to 50 users at once</t>
   </si>
   <si>
-    <t>The server must be up without failure for at least 30 minutes</t>
-  </si>
-  <si>
     <t xml:space="preserve">Users can be muted by other users </t>
   </si>
   <si>
@@ -134,9 +122,6 @@
     <t>Users that do not type something within 300 seconds will be kicked</t>
   </si>
   <si>
-    <t>Any keystroke will reset the timer that does the afk kick</t>
-  </si>
-  <si>
     <t>There will be an option to broadcast a message to all chatrooms</t>
   </si>
   <si>
@@ -152,9 +137,6 @@
     <t>Group</t>
   </si>
   <si>
-    <t>Email</t>
-  </si>
-  <si>
     <t>Function</t>
   </si>
   <si>
@@ -321,6 +303,102 @@
   </si>
   <si>
     <t>'/transfer'||(figure out how to send files using asio)</t>
+  </si>
+  <si>
+    <t>001</t>
+  </si>
+  <si>
+    <t>002</t>
+  </si>
+  <si>
+    <t>003</t>
+  </si>
+  <si>
+    <t>004</t>
+  </si>
+  <si>
+    <t>005</t>
+  </si>
+  <si>
+    <t>006</t>
+  </si>
+  <si>
+    <t>007</t>
+  </si>
+  <si>
+    <t>008</t>
+  </si>
+  <si>
+    <t>009</t>
+  </si>
+  <si>
+    <t>010</t>
+  </si>
+  <si>
+    <t>011</t>
+  </si>
+  <si>
+    <t>012</t>
+  </si>
+  <si>
+    <t>013</t>
+  </si>
+  <si>
+    <t>014</t>
+  </si>
+  <si>
+    <t>015</t>
+  </si>
+  <si>
+    <t>016</t>
+  </si>
+  <si>
+    <t>017</t>
+  </si>
+  <si>
+    <t>018</t>
+  </si>
+  <si>
+    <t>019</t>
+  </si>
+  <si>
+    <t>020</t>
+  </si>
+  <si>
+    <t>021</t>
+  </si>
+  <si>
+    <t>022</t>
+  </si>
+  <si>
+    <t>023</t>
+  </si>
+  <si>
+    <t>024</t>
+  </si>
+  <si>
+    <t>025</t>
+  </si>
+  <si>
+    <t>026</t>
+  </si>
+  <si>
+    <t>027</t>
+  </si>
+  <si>
+    <t>028</t>
+  </si>
+  <si>
+    <t>029</t>
+  </si>
+  <si>
+    <t>030</t>
+  </si>
+  <si>
+    <t>031</t>
+  </si>
+  <si>
+    <t>032</t>
   </si>
 </sst>
 </file>
@@ -459,7 +537,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -488,8 +566,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -512,23 +607,7 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
@@ -612,6 +691,23 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
@@ -769,16 +865,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{25410F8A-371E-0247-A9B9-8551A391583F}" name="Table2" displayName="Table2" ref="A1:G39" totalsRowShown="0" headerRowDxfId="10" dataDxfId="8" headerRowBorderDxfId="9" tableBorderDxfId="7">
-  <autoFilter ref="A1:G39" xr:uid="{F05985FA-B9EA-F449-A6C7-F9E9AA7DABD9}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{25410F8A-371E-0247-A9B9-8551A391583F}" name="Table2" displayName="Table2" ref="A1:G34" totalsRowShown="0" headerRowDxfId="10" dataDxfId="8" headerRowBorderDxfId="9" tableBorderDxfId="7">
+  <autoFilter ref="A1:G34" xr:uid="{F05985FA-B9EA-F449-A6C7-F9E9AA7DABD9}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{D07A80DD-AC43-DA42-ABB9-6917EE1B8195}" name="Identifier" dataDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{A59C9F51-1B73-4D44-BB3C-ADD4E5CA8D26}" name="Requirement" dataDxfId="5"/>
-    <tableColumn id="3" xr3:uid="{894E95CF-9AE1-6D4F-86DF-05B7DDA90BBC}" name="Functional/ Non Functional" dataDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{4D635445-D29B-F04D-BE43-AB8F3A7704C4}" name="Source" dataDxfId="3"/>
-    <tableColumn id="5" xr3:uid="{E60B3A75-156D-F645-AF89-32B86DF5C0B8}" name="Client/Server/Both" dataDxfId="2"/>
-    <tableColumn id="6" xr3:uid="{44E3CF39-3CA5-D746-95A7-BE0099C74661}" name="Notes" dataDxfId="1"/>
-    <tableColumn id="7" xr3:uid="{40A62C7A-29AA-D747-A2D7-F498512DA341}" name="Function" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{D07A80DD-AC43-DA42-ABB9-6917EE1B8195}" name="Identifier" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{A59C9F51-1B73-4D44-BB3C-ADD4E5CA8D26}" name="Requirement" dataDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{894E95CF-9AE1-6D4F-86DF-05B7DDA90BBC}" name="Functional/ Non Functional" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{4D635445-D29B-F04D-BE43-AB8F3A7704C4}" name="Source" dataDxfId="4"/>
+    <tableColumn id="5" xr3:uid="{E60B3A75-156D-F645-AF89-32B86DF5C0B8}" name="Client/Server/Both" dataDxfId="3"/>
+    <tableColumn id="6" xr3:uid="{44E3CF39-3CA5-D746-95A7-BE0099C74661}" name="Notes" dataDxfId="2"/>
+    <tableColumn id="7" xr3:uid="{40A62C7A-29AA-D747-A2D7-F498512DA341}" name="Function" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1081,23 +1177,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3870C74C-FCB0-9F43-AAF6-BFB2D9C0C9DB}">
-  <dimension ref="A1:J39"/>
+  <dimension ref="A1:J38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="G33" sqref="A1:G33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="72" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="58.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25" customWidth="1"/>
-    <col min="5" max="5" width="20.33203125" customWidth="1"/>
+    <col min="1" max="1" width="9" style="16" customWidth="1"/>
+    <col min="2" max="2" width="31.83203125" customWidth="1"/>
+    <col min="3" max="3" width="9" customWidth="1"/>
+    <col min="4" max="4" width="7.83203125" customWidth="1"/>
+    <col min="5" max="5" width="7.33203125" customWidth="1"/>
+    <col min="6" max="6" width="8" customWidth="1"/>
+    <col min="7" max="7" width="16" customWidth="1"/>
+    <col min="8" max="8" width="4" customWidth="1"/>
     <col min="9" max="9" width="5.83203125" customWidth="1"/>
-    <col min="10" max="10" width="20" customWidth="1"/>
+    <col min="10" max="10" width="15.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="72" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
@@ -1116,16 +1217,17 @@
         <v>5</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="I1" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="J1" s="10"/>
+        <v>35</v>
+      </c>
+      <c r="H1" s="10"/>
+      <c r="I1" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="J1" s="11"/>
     </row>
     <row r="2" spans="1:10" ht="72" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="4" t="s">
-        <v>68</v>
+      <c r="A2" s="14" t="s">
+        <v>91</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>6</v>
@@ -1134,24 +1236,27 @@
         <v>7</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>8</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="G2" s="5"/>
-      <c r="I2" s="10" t="s">
-        <v>72</v>
-      </c>
-      <c r="J2" s="10" t="s">
-        <v>73</v>
+      <c r="H2" s="10"/>
+      <c r="I2" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="J2" s="11" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="72" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="4"/>
+      <c r="A3" s="14" t="s">
+        <v>92</v>
+      </c>
       <c r="B3" s="4" t="s">
         <v>9</v>
       </c>
@@ -1159,277 +1264,322 @@
         <v>7</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="E3" s="4" t="s">
         <v>10</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="G3" s="6"/>
-      <c r="I3" s="10" t="s">
-        <v>74</v>
-      </c>
-      <c r="J3" s="10" t="s">
-        <v>75</v>
+      <c r="H3" s="10"/>
+      <c r="I3" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="J3" s="11" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="72" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="6"/>
+      <c r="A4" s="14" t="s">
+        <v>93</v>
+      </c>
       <c r="B4" s="6" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>11</v>
       </c>
       <c r="D4" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="E4" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>45</v>
-      </c>
       <c r="G4" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="I4" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="J4" s="10" t="s">
-        <v>76</v>
+        <v>40</v>
+      </c>
+      <c r="H4" s="10"/>
+      <c r="I4" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="J4" s="11" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="72" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="4"/>
+      <c r="A5" s="14" t="s">
+        <v>94</v>
+      </c>
       <c r="B5" s="4" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>11</v>
       </c>
       <c r="D5" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E5" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>45</v>
-      </c>
       <c r="G5" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="H5" s="10"/>
+      <c r="I5" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="I5" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="J5" s="10" t="s">
-        <v>77</v>
+      <c r="J5" s="11" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="72" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="6"/>
+      <c r="A6" s="14" t="s">
+        <v>95</v>
+      </c>
       <c r="B6" s="6" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="C6" s="6" t="s">
         <v>11</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="E6" s="6" t="s">
         <v>8</v>
       </c>
       <c r="F6" s="1"/>
       <c r="G6" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="I6" s="10" t="s">
-        <v>78</v>
-      </c>
-      <c r="J6" s="10" t="s">
-        <v>82</v>
+        <v>58</v>
+      </c>
+      <c r="H6" s="10"/>
+      <c r="I6" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="J6" s="11" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="72" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="14" t="s">
+        <v>96</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F7" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="H7" s="10"/>
+      <c r="I7" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="J7" s="11" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="72" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G8" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="B7" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F7" s="1"/>
-      <c r="G7" s="6"/>
-      <c r="I7" s="11" t="s">
-        <v>80</v>
-      </c>
-      <c r="J7" s="10" t="s">
+      <c r="H8" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="I8" s="12" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" ht="72" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="6"/>
-      <c r="B8" s="6" t="s">
+      <c r="J8" s="11" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="72" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="B9" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="C8" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="E8" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="F8" s="9" t="s">
-        <v>93</v>
-      </c>
-      <c r="G8" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="H8" t="s">
-        <v>80</v>
-      </c>
-      <c r="I8" s="11" t="s">
-        <v>85</v>
-      </c>
-      <c r="J8" s="10" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" ht="72" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="6"/>
-      <c r="B9" s="6" t="s">
+      <c r="C9" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F9" s="1"/>
+      <c r="G9" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="H9" s="10"/>
+      <c r="I9" s="10"/>
+      <c r="J9" s="10"/>
+    </row>
+    <row r="10" spans="1:10" ht="72" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="14" t="s">
+        <v>99</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F10" s="1"/>
+      <c r="G10" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="H10" s="10"/>
+      <c r="I10" s="10"/>
+      <c r="J10" s="10"/>
+    </row>
+    <row r="11" spans="1:10" ht="72" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="14" t="s">
+        <v>100</v>
+      </c>
+      <c r="B11" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="C9" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="G9" s="6" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" ht="72" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F10" s="1"/>
-      <c r="G10" s="6"/>
-    </row>
-    <row r="11" spans="1:10" ht="72" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="6"/>
-      <c r="B11" s="6" t="s">
-        <v>55</v>
-      </c>
       <c r="C11" s="6" t="s">
         <v>11</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="E11" s="6" t="s">
         <v>8</v>
       </c>
       <c r="F11" s="1"/>
       <c r="G11" s="6" t="s">
-        <v>62</v>
-      </c>
+        <v>53</v>
+      </c>
+      <c r="H11" s="10"/>
+      <c r="I11" s="10"/>
+      <c r="J11" s="10"/>
     </row>
     <row r="12" spans="1:10" ht="72" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="6"/>
+      <c r="A12" s="14" t="s">
+        <v>101</v>
+      </c>
       <c r="B12" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="G12" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="C12" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="E12" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="F12" s="1"/>
-      <c r="G12" s="6" t="s">
-        <v>58</v>
-      </c>
+      <c r="H12" s="10"/>
+      <c r="I12" s="10"/>
+      <c r="J12" s="10"/>
     </row>
     <row r="13" spans="1:10" ht="72" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="6"/>
-      <c r="B13" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>11</v>
+      <c r="A13" s="14" t="s">
+        <v>102</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>7</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="E13" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="F13" s="1"/>
-      <c r="G13" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F13" s="1" t="s">
         <v>59</v>
       </c>
+      <c r="G13" s="6"/>
+      <c r="H13" s="10"/>
+      <c r="I13" s="10"/>
+      <c r="J13" s="10"/>
     </row>
     <row r="14" spans="1:10" ht="72" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="6"/>
-      <c r="B14" s="6" t="s">
+      <c r="A14" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F14" s="1"/>
+      <c r="G14" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="C14" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="E14" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="G14" s="6" t="s">
-        <v>63</v>
-      </c>
+      <c r="H14" s="10"/>
+      <c r="I14" s="10"/>
+      <c r="J14" s="10"/>
     </row>
     <row r="15" spans="1:10" ht="72" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="4" t="s">
-        <v>48</v>
+      <c r="A15" s="14" t="s">
+        <v>104</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>15</v>
@@ -1438,154 +1588,190 @@
         <v>11</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F15" s="1"/>
-      <c r="G15" s="6"/>
+      <c r="G15" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="H15" s="10"/>
+      <c r="I15" s="10"/>
+      <c r="J15" s="10"/>
     </row>
     <row r="16" spans="1:10" ht="72" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="4"/>
-      <c r="B16" s="4" t="s">
+      <c r="A16" s="14" t="s">
+        <v>105</v>
+      </c>
+      <c r="B16" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="C16" s="6" t="s">
         <v>7</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="E16" s="4" t="s">
         <v>10</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="G16" s="6"/>
-    </row>
-    <row r="17" spans="1:7" ht="72" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="4"/>
-      <c r="B17" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="G16" s="8"/>
+      <c r="H16" s="10"/>
+      <c r="I16" s="10"/>
+      <c r="J16" s="10"/>
+    </row>
+    <row r="17" spans="1:10" ht="72" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="B17" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="4" t="s">
-        <v>11</v>
+      <c r="C17" s="6" t="s">
+        <v>7</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="E17" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F17" s="1"/>
-      <c r="G17" s="6" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" ht="72" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="4"/>
-      <c r="B18" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="G17" s="6"/>
+      <c r="H17" s="10"/>
+      <c r="I17" s="10"/>
+      <c r="J17" s="10"/>
+    </row>
+    <row r="18" spans="1:10" ht="72" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="14" t="s">
+        <v>107</v>
+      </c>
+      <c r="B18" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C18" s="4" t="s">
+      <c r="C18" s="6" t="s">
         <v>11</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="E18" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="F18" s="1"/>
+        <v>33</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F18" s="9" t="s">
+        <v>85</v>
+      </c>
       <c r="G18" s="6" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="72" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="6"/>
+        <v>86</v>
+      </c>
+      <c r="H18" s="10"/>
+      <c r="I18" s="10"/>
+      <c r="J18" s="10"/>
+    </row>
+    <row r="19" spans="1:10" ht="72" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="14" t="s">
+        <v>108</v>
+      </c>
       <c r="B19" s="6" t="s">
         <v>19</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="E19" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="G19" s="8"/>
-    </row>
-    <row r="20" spans="1:7" ht="72" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="6"/>
+        <v>33</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F19" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="G19" s="6"/>
+      <c r="H19" s="10"/>
+      <c r="I19" s="10"/>
+      <c r="J19" s="10"/>
+    </row>
+    <row r="20" spans="1:10" ht="72" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="14" t="s">
+        <v>109</v>
+      </c>
       <c r="B20" s="6" t="s">
         <v>20</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>70</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="F20" s="9"/>
       <c r="G20" s="6"/>
-    </row>
-    <row r="21" spans="1:7" ht="72" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="6" t="s">
-        <v>68</v>
+      <c r="H20" s="10"/>
+      <c r="I20" s="10"/>
+      <c r="J20" s="10"/>
+    </row>
+    <row r="21" spans="1:10" ht="72" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="14" t="s">
+        <v>110</v>
       </c>
       <c r="B21" s="6" t="s">
         <v>21</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F21" s="1"/>
-      <c r="G21" s="6"/>
-    </row>
-    <row r="22" spans="1:7" ht="72" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="6" t="s">
-        <v>68</v>
+        <v>8</v>
+      </c>
+      <c r="F21" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="G21" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="H21" s="10"/>
+      <c r="I21" s="10"/>
+      <c r="J21" s="10"/>
+    </row>
+    <row r="22" spans="1:10" ht="72" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="14" t="s">
+        <v>111</v>
       </c>
       <c r="B22" s="6" t="s">
         <v>22</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="F22" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="G22" s="6" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" ht="72" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="6" t="s">
-        <v>68</v>
+        <v>12</v>
+      </c>
+      <c r="F22" s="1"/>
+      <c r="G22" s="6"/>
+      <c r="H22" s="10"/>
+      <c r="I22" s="10"/>
+      <c r="J22" s="10"/>
+    </row>
+    <row r="23" spans="1:10" ht="72" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="14" t="s">
+        <v>112</v>
       </c>
       <c r="B23" s="6" t="s">
         <v>23</v>
@@ -1594,19 +1780,20 @@
         <v>11</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="F23" s="9" t="s">
-        <v>96</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="F23" s="1"/>
       <c r="G23" s="6"/>
-    </row>
-    <row r="24" spans="1:7" ht="72" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="6" t="s">
-        <v>68</v>
+      <c r="H23" s="10"/>
+      <c r="I23" s="10"/>
+      <c r="J23" s="10"/>
+    </row>
+    <row r="24" spans="1:10" ht="72" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="14" t="s">
+        <v>113</v>
       </c>
       <c r="B24" s="6" t="s">
         <v>24</v>
@@ -1615,173 +1802,208 @@
         <v>11</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="E24" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="F24" s="9"/>
+      <c r="F24" s="1" t="s">
+        <v>77</v>
+      </c>
       <c r="G24" s="6"/>
-    </row>
-    <row r="25" spans="1:7" ht="72" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="6"/>
+      <c r="H24" s="10"/>
+      <c r="I24" s="10"/>
+      <c r="J24" s="10"/>
+    </row>
+    <row r="25" spans="1:10" ht="72" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="14" t="s">
+        <v>114</v>
+      </c>
       <c r="B25" s="6" t="s">
         <v>25</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="E25" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="F25" s="9" t="s">
-        <v>86</v>
-      </c>
-      <c r="G25" s="6" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" ht="72" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="6"/>
+      <c r="F25" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="G25" s="6"/>
+      <c r="H25" s="10"/>
+      <c r="I25" s="10"/>
+      <c r="J25" s="10"/>
+    </row>
+    <row r="26" spans="1:10" ht="72" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="14" t="s">
+        <v>115</v>
+      </c>
       <c r="B26" s="6" t="s">
         <v>26</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="E26" s="6" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F26" s="1"/>
       <c r="G26" s="6"/>
-    </row>
-    <row r="27" spans="1:7" ht="72" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="6" t="s">
-        <v>68</v>
+      <c r="H26" s="10"/>
+      <c r="I26" s="10"/>
+      <c r="J26" s="10"/>
+    </row>
+    <row r="27" spans="1:10" ht="72" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="14" t="s">
+        <v>116</v>
       </c>
       <c r="B27" s="6" t="s">
         <v>27</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="E27" s="6" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F27" s="1"/>
       <c r="G27" s="6"/>
-    </row>
-    <row r="28" spans="1:7" ht="72" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="6" t="s">
-        <v>68</v>
+      <c r="H27" s="10"/>
+      <c r="I27" s="10"/>
+      <c r="J27" s="10"/>
+    </row>
+    <row r="28" spans="1:10" ht="72" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="14" t="s">
+        <v>117</v>
       </c>
       <c r="B28" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="C28" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E28" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F28" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="G28" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="H28" s="10"/>
+      <c r="I28" s="10"/>
+      <c r="J28" s="10"/>
+    </row>
+    <row r="29" spans="1:10" ht="72" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="14" t="s">
+        <v>118</v>
+      </c>
+      <c r="B29" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="C28" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="E28" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="F28" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="G28" s="6"/>
-    </row>
-    <row r="29" spans="1:7" ht="72" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="B29" s="6" t="s">
+      <c r="C29" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E29" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F29" s="1"/>
+      <c r="G29" s="6"/>
+      <c r="H29" s="10"/>
+      <c r="I29" s="10"/>
+      <c r="J29" s="10"/>
+    </row>
+    <row r="30" spans="1:10" ht="72" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="14" t="s">
+        <v>119</v>
+      </c>
+      <c r="B30" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="C29" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="E29" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="F29" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="G29" s="6"/>
-    </row>
-    <row r="30" spans="1:7" ht="72" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="B30" s="6" t="s">
-        <v>30</v>
-      </c>
       <c r="C30" s="6" t="s">
         <v>11</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="E30" s="6" t="s">
         <v>8</v>
       </c>
       <c r="F30" s="1"/>
       <c r="G30" s="6"/>
-    </row>
-    <row r="31" spans="1:7" ht="72" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="6"/>
+      <c r="H30" s="10"/>
+      <c r="I30" s="10"/>
+      <c r="J30" s="10"/>
+    </row>
+    <row r="31" spans="1:10" ht="72" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="14" t="s">
+        <v>120</v>
+      </c>
       <c r="B31" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C31" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E31" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F31" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="G31" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="H31" s="10"/>
+      <c r="I31" s="10"/>
+      <c r="J31" s="10"/>
+    </row>
+    <row r="32" spans="1:10" ht="72" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="B32" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="C31" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="E31" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="F31" s="1"/>
-      <c r="G31" s="6"/>
-    </row>
-    <row r="32" spans="1:7" ht="72" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="6"/>
-      <c r="B32" s="6" t="s">
-        <v>84</v>
-      </c>
       <c r="C32" s="6" t="s">
         <v>11</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="E32" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="F32" s="9" t="s">
-        <v>87</v>
-      </c>
-      <c r="G32" s="6" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" ht="72" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="6" t="s">
-        <v>68</v>
+        <v>10</v>
+      </c>
+      <c r="F32" s="1"/>
+      <c r="G32" s="6"/>
+      <c r="H32" s="10"/>
+      <c r="I32" s="10"/>
+      <c r="J32" s="10"/>
+    </row>
+    <row r="33" spans="1:10" ht="72" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="14" t="s">
+        <v>122</v>
       </c>
       <c r="B33" s="6" t="s">
         <v>32</v>
@@ -1790,117 +2012,48 @@
         <v>11</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="E33" s="6" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F33" s="1"/>
       <c r="G33" s="6"/>
-    </row>
-    <row r="34" spans="1:7" ht="72" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="B34" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="C34" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="E34" s="6" t="s">
-        <v>8</v>
-      </c>
+      <c r="H33" s="10"/>
+      <c r="I33" s="10"/>
+      <c r="J33" s="10"/>
+    </row>
+    <row r="34" spans="1:10" ht="72" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="15"/>
+      <c r="B34" s="1"/>
+      <c r="C34" s="1"/>
+      <c r="D34" s="1"/>
+      <c r="E34" s="1"/>
       <c r="F34" s="1"/>
-      <c r="G34" s="6"/>
-    </row>
-    <row r="35" spans="1:7" ht="72" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="6"/>
-      <c r="B35" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="C35" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="D35" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="E35" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="F35" s="1"/>
-      <c r="G35" s="6"/>
-    </row>
-    <row r="36" spans="1:7" ht="72" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="6"/>
-      <c r="B36" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="C36" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="D36" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="E36" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="F36" s="9" t="s">
-        <v>94</v>
-      </c>
-      <c r="G36" s="6" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" ht="72" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="B37" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="C37" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="E37" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F37" s="1"/>
-      <c r="G37" s="6"/>
-    </row>
-    <row r="38" spans="1:7" ht="72" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="B38" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="C38" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="D38" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="E38" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="F38" s="1"/>
-      <c r="G38" s="6"/>
-    </row>
-    <row r="39" spans="1:7" ht="72" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="6"/>
-      <c r="B39" s="1"/>
-      <c r="C39" s="1"/>
-      <c r="D39" s="1"/>
-      <c r="E39" s="1"/>
-      <c r="F39" s="1"/>
-      <c r="G39" s="7"/>
+      <c r="G34" s="7"/>
+      <c r="H34" s="10"/>
+      <c r="I34" s="10"/>
+      <c r="J34" s="10"/>
+    </row>
+    <row r="35" spans="1:10" ht="72" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H35" s="10"/>
+      <c r="I35" s="10"/>
+      <c r="J35" s="10"/>
+    </row>
+    <row r="36" spans="1:10" ht="72" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H36" s="10"/>
+      <c r="I36" s="10"/>
+      <c r="J36" s="10"/>
+    </row>
+    <row r="37" spans="1:10" ht="72" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H37" s="10"/>
+      <c r="I37" s="10"/>
+      <c r="J37" s="10"/>
+    </row>
+    <row r="38" spans="1:10" ht="72" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H38" s="10"/>
+      <c r="I38" s="10"/>
+      <c r="J38" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>